<commit_message>
Spring Security Day 2
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/produk.xlsx
+++ b/src/main/resources/excel/produk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Batch26\pcmspringboot4\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B55B6B9-74BC-49FE-AEEA-9B75D782301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0D9FEA-6B75-4674-8506-C4A39130C0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{47EA533E-3F0C-4ED1-A111-B65235F9FF84}"/>
   </bookViews>
@@ -20,25 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
-  <si>
-    <t>Nama Produk</t>
-  </si>
-  <si>
-    <t>Deskripsi Produk</t>
-  </si>
-  <si>
-    <t>Merk</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Stok</t>
-  </si>
-  <si>
-    <t>Kategori</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Produk1</t>
   </si>
@@ -146,6 +128,54 @@
   </si>
   <si>
     <t>Model9</t>
+  </si>
+  <si>
+    <t>NAMA PRODUK</t>
+  </si>
+  <si>
+    <t>DESKRIPSI PRODUK</t>
+  </si>
+  <si>
+    <t>MERK</t>
+  </si>
+  <si>
+    <t>MODEL</t>
+  </si>
+  <si>
+    <t>STOK</t>
+  </si>
+  <si>
+    <t>KATEGORI</t>
+  </si>
+  <si>
+    <t>WARNA</t>
+  </si>
+  <si>
+    <t>Merah Marun1</t>
+  </si>
+  <si>
+    <t>Merah Marun2</t>
+  </si>
+  <si>
+    <t>Merah Marun3</t>
+  </si>
+  <si>
+    <t>Merah Marun4</t>
+  </si>
+  <si>
+    <t>Merah Marun5</t>
+  </si>
+  <si>
+    <t>Merah Marun6</t>
+  </si>
+  <si>
+    <t>Merah Marun7</t>
+  </si>
+  <si>
+    <t>Merah Marun8</t>
+  </si>
+  <si>
+    <t>Merah Marun9</t>
   </si>
 </sst>
 </file>
@@ -992,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B721B2D5-CAB4-497F-A89F-1920D5BE88DB}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1005,38 +1035,41 @@
     <col min="3" max="3" width="20.921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>51</v>
@@ -1044,165 +1077,192 @@
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E4">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E5">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E6">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E7">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F7">
         <v>3</v>
       </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E8">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E9">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E10">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F10">
         <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>